<commit_message>
Changes made to the file
</commit_message>
<xml_diff>
--- a/Excel Formulas.xlsx
+++ b/Excel Formulas.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROJECTOG\DANLC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B5C5C7CE-9214-4BF8-80A1-3D1E48CF38C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97AEF7D1-2179-49B3-87B2-355A533E149D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{06559643-08B1-46AF-98FA-A483CEC93FE2}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t xml:space="preserve">Basic Excel Formulas </t>
   </si>
@@ -57,18 +57,6 @@
     <t>Yash</t>
   </si>
   <si>
-    <t xml:space="preserve">Sahil  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Siddesh  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chinnmay </t>
-  </si>
-  <si>
-    <t>Umesh</t>
-  </si>
-  <si>
     <t>Parag</t>
   </si>
   <si>
@@ -184,6 +172,21 @@
   </si>
   <si>
     <t>Median=&gt;</t>
+  </si>
+  <si>
+    <t>Fairaaz</t>
+  </si>
+  <si>
+    <t>Uday</t>
+  </si>
+  <si>
+    <t>Pratham</t>
+  </si>
+  <si>
+    <t>Siddharth</t>
+  </si>
+  <si>
+    <t>Atharva</t>
   </si>
 </sst>
 </file>
@@ -611,7 +614,7 @@
   <dimension ref="B1:H38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -651,13 +654,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>7</v>
+        <v>46</v>
       </c>
       <c r="D4" s="4">
         <v>21</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F4" s="4">
         <v>25000</v>
@@ -668,13 +671,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>8</v>
+        <v>49</v>
       </c>
       <c r="D5" s="4">
         <v>26</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="F5" s="4">
         <v>35000</v>
@@ -691,7 +694,7 @@
         <v>58</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F6" s="4">
         <v>26000</v>
@@ -702,13 +705,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>9</v>
+        <v>50</v>
       </c>
       <c r="D7" s="4">
         <v>25</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F7" s="4">
         <v>40000</v>
@@ -719,13 +722,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>10</v>
+        <v>47</v>
       </c>
       <c r="D8" s="4">
         <v>24</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F8" s="4">
         <v>37000</v>
@@ -736,13 +739,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="D9" s="4">
         <v>30</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F9" s="4">
         <v>40000</v>
@@ -753,13 +756,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D10" s="4">
         <v>35</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="F10" s="4">
         <v>23000</v>
@@ -770,13 +773,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D11" s="4">
         <v>22</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F11" s="4">
         <v>40000</v>
@@ -787,13 +790,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D12" s="4">
         <v>27</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F12" s="4">
         <v>45000</v>
@@ -804,13 +807,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D13" s="4">
         <v>35</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F13" s="4">
         <v>20000</v>
@@ -818,14 +821,14 @@
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D16" s="5" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E16">
         <f>SUM(F4:F13)</f>
         <v>331000</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="H16">
         <f>AVERAGE(F4:F13)</f>
@@ -834,14 +837,14 @@
     </row>
     <row r="17" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D17" s="5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E17">
         <f>SUMIF(F4:F13,"&gt;40000")</f>
         <v>45000</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="H17">
         <f>MEDIAN(F4:F13)</f>
@@ -850,7 +853,7 @@
     </row>
     <row r="18" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D18" s="5" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E18">
         <f>MIN(F4:F13)</f>
@@ -860,7 +863,7 @@
     </row>
     <row r="19" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D19" s="5" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E19">
         <f>MAX(F4:F13)</f>
@@ -869,7 +872,7 @@
     </row>
     <row r="20" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D20" s="5" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E20">
         <f>AVERAGE(F4:F13)</f>
@@ -878,7 +881,7 @@
     </row>
     <row r="21" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D21" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E21">
         <f>COUNT(D4:D13)</f>
@@ -887,7 +890,7 @@
     </row>
     <row r="22" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D22" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E22">
         <f>COUNTBLANK(F4:F13)</f>
@@ -896,7 +899,7 @@
     </row>
     <row r="23" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D23" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E23">
         <f>POWER(D5,2)</f>
@@ -905,7 +908,7 @@
     </row>
     <row r="24" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D24" s="5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E24" t="str">
         <f>_xlfn.CONCAT(C6,E6)</f>
@@ -914,7 +917,7 @@
     </row>
     <row r="25" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D25" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E25" t="str">
         <f>TRIM(E11)</f>
@@ -923,7 +926,7 @@
     </row>
     <row r="26" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D26" s="5" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E26" t="str">
         <f>REPLACE(C11,1,1,"K")</f>
@@ -932,7 +935,7 @@
     </row>
     <row r="27" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D27" s="5" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E27" t="str">
         <f>LEFT(E8,8)</f>
@@ -941,7 +944,7 @@
     </row>
     <row r="28" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D28" s="5" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E28" t="str">
         <f>MID(E12,6,8)</f>
@@ -950,7 +953,7 @@
     </row>
     <row r="29" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D29" s="5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E29" t="str">
         <f>RIGHT(E5,3)</f>
@@ -959,7 +962,7 @@
     </row>
     <row r="30" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D30" s="5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E30" t="str">
         <f>UPPER(E10)</f>
@@ -968,7 +971,7 @@
     </row>
     <row r="31" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D31" s="5" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E31" t="str">
         <f>LOWER(E12)</f>
@@ -977,16 +980,16 @@
     </row>
     <row r="32" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D32" s="5" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E32" s="7">
         <f ca="1">NOW()</f>
-        <v>45506.451521064817</v>
+        <v>45506.469016898147</v>
       </c>
     </row>
     <row r="33" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D33" s="5" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E33">
         <f ca="1">DAY((TODAY()))</f>
@@ -995,7 +998,7 @@
     </row>
     <row r="34" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D34" s="5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E34">
         <f ca="1">MONTH((TODAY()))</f>
@@ -1004,7 +1007,7 @@
     </row>
     <row r="35" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D35" s="5" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E35">
         <f ca="1">YEAR(TODAY())</f>
@@ -1013,7 +1016,7 @@
     </row>
     <row r="36" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D36" s="5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E36" t="str">
         <f>IF(D7&gt;30,"HR","Developer")</f>
@@ -1022,7 +1025,7 @@
     </row>
     <row r="37" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D37" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E37" t="str">
         <f>INDEX(E4:E13,9)</f>
@@ -1031,7 +1034,7 @@
     </row>
     <row r="38" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D38" s="6" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E38">
         <f>MATCH(F7,F11:F13)</f>

</xml_diff>